<commit_message>
Updated Project Manager file
</commit_message>
<xml_diff>
--- a/docs/Project Manager Template.xlsx
+++ b/docs/Project Manager Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psnpo\OneDrive - Concord University\Documents\Concord\CS 456\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psnpo\Documents\GitHub\video-player\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E882A1E0-F3D3-4A58-94FC-AFFEAD13D188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D09912-BC1E-4A67-992B-E5A66D7BB33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Major Tasks</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Owner / Priority</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
     <t>Alt +</t>
   </si>
   <si>
@@ -46,22 +43,64 @@
     <t>™</t>
   </si>
   <si>
-    <t>Date: mm/dd/yy</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Project Objective: </t>
+      <t xml:space="preserve">Project Completed By: </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color indexed="22"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>text</t>
+      <t>date</t>
     </r>
+  </si>
+  <si>
+    <t>Oct 1-15</t>
+  </si>
+  <si>
+    <t>Oct 16-31</t>
+  </si>
+  <si>
+    <t>Nov 1-15</t>
+  </si>
+  <si>
+    <t>Nov 16-30</t>
+  </si>
+  <si>
+    <t>Dec 1-15</t>
+  </si>
+  <si>
+    <t>Jan 1-15</t>
+  </si>
+  <si>
+    <t>Jan 16-31</t>
+  </si>
+  <si>
+    <t>Feb 1-15</t>
+  </si>
+  <si>
+    <t>Feb 16-28</t>
+  </si>
+  <si>
+    <t>Mar 1-15</t>
+  </si>
+  <si>
+    <t>Mar 16-30</t>
+  </si>
+  <si>
+    <t>Apr 1-15</t>
+  </si>
+  <si>
+    <t>Ashton</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>Mikel</t>
   </si>
   <si>
     <r>
@@ -75,7 +114,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>name</t>
+      <t>Logan Z</t>
     </r>
   </si>
   <si>
@@ -90,83 +129,67 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Project Completed By: </t>
+      <t>Z</t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color indexed="22"/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FFC0C0C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>date</t>
+      <t>2</t>
     </r>
   </si>
   <si>
-    <t>Oct 1-15</t>
-  </si>
-  <si>
-    <t>Oct 16-31</t>
-  </si>
-  <si>
-    <t>Nov 1-15</t>
-  </si>
-  <si>
-    <t>Nov 16-30</t>
-  </si>
-  <si>
-    <t>Dec 1-15</t>
-  </si>
-  <si>
-    <t>Jan 1-15</t>
-  </si>
-  <si>
-    <t>Jan 16-31</t>
-  </si>
-  <si>
-    <t>Feb 1-15</t>
-  </si>
-  <si>
-    <t>Feb 16-28</t>
-  </si>
-  <si>
-    <t>Mar 1-15</t>
-  </si>
-  <si>
-    <t>Mar 16-30</t>
-  </si>
-  <si>
-    <t>Apr 1-15</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Project Team: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color indexed="22"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>name(s)</t>
-    </r>
-  </si>
-  <si>
-    <t>Ashton</t>
-  </si>
-  <si>
-    <t>Hunter</t>
-  </si>
-  <si>
-    <t>Mikel</t>
+    <t>Project Team: Logan Z, Hunter, Mikel, Ashton, Zach</t>
+  </si>
+  <si>
+    <t>Video Player</t>
+  </si>
+  <si>
+    <t>Page Layout</t>
+  </si>
+  <si>
+    <t>Page Banner</t>
+  </si>
+  <si>
+    <t>Separate tabs (demo)</t>
+  </si>
+  <si>
+    <t>Database for acounts</t>
+  </si>
+  <si>
+    <t>Accounts/Login Page</t>
+  </si>
+  <si>
+    <t>Minor functionality of other tabs</t>
+  </si>
+  <si>
+    <t>Categories (Subjects + Searching)</t>
+  </si>
+  <si>
+    <t>Flesh out navigation</t>
+  </si>
+  <si>
+    <t>Video Uploading</t>
+  </si>
+  <si>
+    <t>Account Personalization</t>
+  </si>
+  <si>
+    <t>Logan Z</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Project Objective: Create a video sharing website</t>
+  </si>
+  <si>
+    <t>Date: 10/02/24</t>
   </si>
 </sst>
 </file>
@@ -237,13 +260,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color indexed="22"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color indexed="22"/>
       <name val="Arial"/>
@@ -256,6 +272,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color rgb="FFC0C0C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -265,7 +289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -774,21 +798,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -865,6 +874,90 @@
       </top>
       <bottom style="hair">
         <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="22"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="22"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </right>
+      <top style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </left>
+      <right style="hair">
+        <color indexed="22"/>
+      </right>
+      <top style="hair">
+        <color indexed="22"/>
+      </top>
+      <bottom style="hair">
+        <color theme="0" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -874,7 +967,7 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -950,10 +1043,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1088,10 +1177,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="47" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="46" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1102,6 +1191,60 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1135,14 +1278,6 @@
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="17" fontId="5" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
@@ -1163,64 +1298,50 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1846,7 +1967,7 @@
   <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="73" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27:T32"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1866,25 +1987,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:25" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="101"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="J2" s="68"/>
       <c r="K2" s="8"/>
-      <c r="L2" s="101"/>
+      <c r="L2" s="68"/>
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
@@ -1894,94 +2013,96 @@
       <c r="S2" s="11"/>
       <c r="T2" s="11"/>
       <c r="U2" s="12" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="W2" s="13"/>
       <c r="X2" s="14"/>
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="84" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="M3" s="85"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
-      <c r="P3" s="85"/>
-      <c r="Q3" s="85"/>
-      <c r="R3" s="85"/>
-      <c r="S3" s="85"/>
-      <c r="T3" s="85"/>
-      <c r="U3" s="86"/>
+      <c r="A3" s="69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="97"/>
+      <c r="U3" s="98"/>
       <c r="W3" s="13"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="87"/>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="89"/>
+      <c r="A4" s="70"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="103"/>
+      <c r="F4" s="103"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="103"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
+      <c r="M4" s="103"/>
+      <c r="N4" s="103"/>
+      <c r="O4" s="103"/>
+      <c r="P4" s="103"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="99"/>
+      <c r="U4" s="100"/>
       <c r="W4" s="16"/>
       <c r="X4" s="17"/>
       <c r="Y4" s="17"/>
     </row>
     <row r="5" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="19"/>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="64" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="96" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
-      <c r="K5" s="97"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="98"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="100" t="s">
+      <c r="E5" s="105" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="97"/>
-      <c r="S5" s="97"/>
-      <c r="T5" s="97"/>
-      <c r="U5" s="99"/>
+      <c r="R5" s="80"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="82"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -1990,867 +2111,929 @@
       <c r="A6" s="24">
         <v>1</v>
       </c>
-      <c r="B6" s="25"/>
+      <c r="B6" s="25" t="s">
+        <v>25</v>
+      </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="32"/>
-      <c r="W6" s="33"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
+      <c r="E6" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="104"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="31"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
     </row>
     <row r="7" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="34">
         <v>2</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="42"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="43"/>
-      <c r="W7" s="33"/>
-      <c r="X7" s="34"/>
-      <c r="Y7" s="34"/>
+      <c r="B7" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="108" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="42"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="33"/>
+      <c r="Y7" s="33"/>
     </row>
     <row r="8" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
+      <c r="A8" s="34">
         <v>3</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="40"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="42"/>
-      <c r="S8" s="42"/>
-      <c r="T8" s="42"/>
-      <c r="U8" s="43"/>
-      <c r="W8" s="33"/>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="34"/>
+      <c r="B8" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="108" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="42"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="33"/>
+      <c r="Y8" s="33"/>
     </row>
     <row r="9" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35">
+      <c r="A9" s="34">
         <v>4</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="42"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="43"/>
-      <c r="W9" s="33"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="34"/>
+      <c r="B9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="106"/>
+      <c r="F9" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="42"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="33"/>
+      <c r="Y9" s="33"/>
     </row>
     <row r="10" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
+      <c r="A10" s="34">
         <v>5</v>
       </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="42"/>
-      <c r="S10" s="42"/>
-      <c r="T10" s="42"/>
-      <c r="U10" s="43"/>
-      <c r="W10" s="33"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="34"/>
+      <c r="B10" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="42"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="33"/>
+      <c r="Y10" s="33"/>
     </row>
     <row r="11" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35">
+      <c r="A11" s="34">
         <v>6</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="42"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="43"/>
-      <c r="W11" s="33"/>
-      <c r="X11" s="34"/>
-      <c r="Y11" s="34"/>
+      <c r="B11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="39"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="42"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="33"/>
+      <c r="Y11" s="33"/>
     </row>
     <row r="12" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35">
+      <c r="A12" s="34">
         <v>7</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="43"/>
-      <c r="W12" s="33"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="34"/>
+      <c r="B12" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="39"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="42"/>
+      <c r="W12" s="32"/>
+      <c r="X12" s="33"/>
+      <c r="Y12" s="33"/>
     </row>
     <row r="13" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
+      <c r="A13" s="34">
         <v>8</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
-      <c r="U13" s="43"/>
-      <c r="W13" s="33"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="34"/>
+      <c r="B13" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="42"/>
+      <c r="W13" s="32"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
     </row>
     <row r="14" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35">
+      <c r="A14" s="34">
         <v>9</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="42"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="43"/>
-      <c r="W14" s="33"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="34"/>
+      <c r="B14" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="42"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
     </row>
     <row r="15" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35">
+      <c r="A15" s="34">
         <v>10</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="41"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="43"/>
-      <c r="W15" s="33"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="34"/>
+      <c r="B15" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="42"/>
+      <c r="W15" s="32"/>
+      <c r="X15" s="33"/>
+      <c r="Y15" s="33"/>
     </row>
     <row r="16" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
+      <c r="A16" s="34">
         <v>11</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="41"/>
-      <c r="R16" s="42"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="43"/>
-      <c r="W16" s="33"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="34"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="42"/>
+      <c r="W16" s="32"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
     </row>
     <row r="17" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35">
+      <c r="A17" s="34">
         <v>12</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="42"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="43"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="34"/>
+      <c r="B17" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="109" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="42"/>
+      <c r="W17" s="32"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
     </row>
     <row r="18" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35">
+      <c r="A18" s="34">
         <v>13</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
-      <c r="U18" s="43"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="42"/>
+      <c r="W18" s="32"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
     </row>
     <row r="19" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35">
+      <c r="A19" s="34">
         <v>14</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="40"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="42"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="43"/>
-      <c r="W19" s="33"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="34"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="42"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
     </row>
     <row r="20" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35">
+      <c r="A20" s="34">
         <v>15</v>
       </c>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
-      <c r="U20" s="43"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="42"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
     </row>
     <row r="21" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35">
+      <c r="A21" s="34">
         <v>16</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="43"/>
-      <c r="W21" s="33"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="34"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="42"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="33"/>
+      <c r="Y21" s="33"/>
     </row>
     <row r="22" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
+      <c r="A22" s="34">
         <v>17</v>
       </c>
-      <c r="B22" s="44"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="43"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="42"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="33"/>
+      <c r="Y22" s="33"/>
     </row>
     <row r="23" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35">
+      <c r="A23" s="34">
         <v>18</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
-      <c r="P23" s="40"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="42"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="43"/>
-      <c r="W23" s="33"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="34"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="41"/>
+      <c r="T23" s="41"/>
+      <c r="U23" s="42"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="33"/>
+      <c r="Y23" s="33"/>
     </row>
     <row r="24" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35">
+      <c r="A24" s="34">
         <v>19</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="42"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="43"/>
-      <c r="W24" s="33"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="34"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="41"/>
+      <c r="T24" s="41"/>
+      <c r="U24" s="42"/>
+      <c r="W24" s="32"/>
+      <c r="X24" s="33"/>
+      <c r="Y24" s="33"/>
     </row>
     <row r="25" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35">
+      <c r="A25" s="34">
         <v>20</v>
       </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="42"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
-      <c r="U25" s="43"/>
-      <c r="W25" s="33"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="34"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
+      <c r="T25" s="41"/>
+      <c r="U25" s="42"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="33"/>
+      <c r="Y25" s="33"/>
     </row>
     <row r="26" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="52"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="53"/>
-      <c r="T26" s="53"/>
-      <c r="U26" s="54"/>
-      <c r="W26" s="33"/>
-      <c r="X26" s="34"/>
-      <c r="Y26" s="34"/>
+      <c r="A26" s="45"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="52"/>
+      <c r="S26" s="52"/>
+      <c r="T26" s="52"/>
+      <c r="U26" s="53"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="33"/>
+      <c r="Y26" s="33"/>
     </row>
     <row r="27" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="94" t="s">
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="78" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="77" t="s">
+      <c r="K27" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="77" t="s">
+      <c r="L27" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="H27" s="77" t="s">
+      <c r="M27" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="77" t="s">
+      <c r="N27" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="77" t="s">
+      <c r="O27" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="77" t="s">
+      <c r="P27" s="92" t="s">
         <v>18</v>
       </c>
-      <c r="L27" s="77" t="s">
+      <c r="Q27" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="M27" s="77" t="s">
+      <c r="R27" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="N27" s="77" t="s">
+      <c r="S27" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="O27" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="P27" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q27" s="92" t="s">
-        <v>25</v>
-      </c>
-      <c r="R27" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="S27" s="75" t="s">
-        <v>27</v>
-      </c>
-      <c r="T27" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="U27" s="90" t="s">
-        <v>2</v>
-      </c>
-      <c r="W27" s="33"/>
-      <c r="X27" s="34"/>
-      <c r="Y27" s="34"/>
+      <c r="T27" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="U27" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="W27" s="32"/>
+      <c r="X27" s="33"/>
+      <c r="Y27" s="33"/>
     </row>
     <row r="28" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="55"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="77"/>
-      <c r="J28" s="77"/>
-      <c r="K28" s="77"/>
-      <c r="L28" s="77"/>
-      <c r="M28" s="77"/>
-      <c r="N28" s="77"/>
-      <c r="O28" s="77"/>
-      <c r="P28" s="79"/>
-      <c r="Q28" s="92"/>
-      <c r="R28" s="75"/>
-      <c r="S28" s="75"/>
-      <c r="T28" s="75"/>
-      <c r="U28" s="90"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="34"/>
-      <c r="Y28" s="34"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="76"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="76"/>
+      <c r="K28" s="76"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="76"/>
+      <c r="O28" s="76"/>
+      <c r="P28" s="92"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="90"/>
+      <c r="S28" s="90"/>
+      <c r="T28" s="90"/>
+      <c r="U28" s="72"/>
+      <c r="W28" s="32"/>
+      <c r="X28" s="33"/>
+      <c r="Y28" s="33"/>
     </row>
     <row r="29" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="55"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="77"/>
-      <c r="J29" s="77"/>
-      <c r="K29" s="77"/>
-      <c r="L29" s="77"/>
-      <c r="M29" s="77"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="77"/>
-      <c r="P29" s="79"/>
-      <c r="Q29" s="92"/>
-      <c r="R29" s="75"/>
-      <c r="S29" s="75"/>
-      <c r="T29" s="75"/>
-      <c r="U29" s="90"/>
-      <c r="W29" s="33"/>
-      <c r="X29" s="34"/>
-      <c r="Y29" s="34"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="76"/>
+      <c r="I29" s="76"/>
+      <c r="J29" s="76"/>
+      <c r="K29" s="76"/>
+      <c r="L29" s="76"/>
+      <c r="M29" s="76"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="76"/>
+      <c r="P29" s="92"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="90"/>
+      <c r="S29" s="90"/>
+      <c r="T29" s="90"/>
+      <c r="U29" s="72"/>
+      <c r="W29" s="32"/>
+      <c r="X29" s="33"/>
+      <c r="Y29" s="33"/>
     </row>
     <row r="30" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="55"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="77"/>
-      <c r="J30" s="77"/>
-      <c r="K30" s="77"/>
-      <c r="L30" s="77"/>
-      <c r="M30" s="77"/>
-      <c r="N30" s="77"/>
-      <c r="O30" s="77"/>
-      <c r="P30" s="79"/>
-      <c r="Q30" s="92"/>
-      <c r="R30" s="75"/>
-      <c r="S30" s="75"/>
-      <c r="T30" s="75"/>
-      <c r="U30" s="90"/>
-      <c r="X30" s="34"/>
-      <c r="Y30" s="34"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="76"/>
+      <c r="J30" s="76"/>
+      <c r="K30" s="76"/>
+      <c r="L30" s="76"/>
+      <c r="M30" s="76"/>
+      <c r="N30" s="76"/>
+      <c r="O30" s="76"/>
+      <c r="P30" s="92"/>
+      <c r="Q30" s="74"/>
+      <c r="R30" s="90"/>
+      <c r="S30" s="90"/>
+      <c r="T30" s="90"/>
+      <c r="U30" s="72"/>
+      <c r="X30" s="33"/>
+      <c r="Y30" s="33"/>
     </row>
     <row r="31" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="55"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="94"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="77"/>
-      <c r="M31" s="77"/>
-      <c r="N31" s="77"/>
-      <c r="O31" s="77"/>
-      <c r="P31" s="79"/>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="75"/>
-      <c r="S31" s="75"/>
-      <c r="T31" s="75"/>
-      <c r="U31" s="90"/>
-      <c r="X31" s="34"/>
-      <c r="Y31" s="34"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="76"/>
+      <c r="J31" s="76"/>
+      <c r="K31" s="76"/>
+      <c r="L31" s="76"/>
+      <c r="M31" s="76"/>
+      <c r="N31" s="76"/>
+      <c r="O31" s="76"/>
+      <c r="P31" s="92"/>
+      <c r="Q31" s="74"/>
+      <c r="R31" s="90"/>
+      <c r="S31" s="90"/>
+      <c r="T31" s="90"/>
+      <c r="U31" s="72"/>
+      <c r="X31" s="33"/>
+      <c r="Y31" s="33"/>
     </row>
     <row r="32" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="55"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="95"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-      <c r="O32" s="78"/>
-      <c r="P32" s="80"/>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="76"/>
-      <c r="S32" s="76"/>
-      <c r="T32" s="76"/>
-      <c r="U32" s="91"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="79"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="93"/>
+      <c r="Q32" s="75"/>
+      <c r="R32" s="91"/>
+      <c r="S32" s="91"/>
+      <c r="T32" s="91"/>
+      <c r="U32" s="73"/>
       <c r="W32" s="21"/>
       <c r="X32" s="21"/>
       <c r="Y32" s="21"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="81"/>
-      <c r="B33" s="82"/>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="82"/>
-      <c r="H33" s="82"/>
-      <c r="I33" s="82"/>
-      <c r="J33" s="82"/>
-      <c r="K33" s="82"/>
-      <c r="L33" s="82"/>
-      <c r="M33" s="82"/>
-      <c r="N33" s="82"/>
-      <c r="O33" s="82"/>
-      <c r="P33" s="82"/>
-      <c r="Q33" s="82"/>
-      <c r="R33" s="82"/>
-      <c r="S33" s="82"/>
-      <c r="T33" s="82"/>
-      <c r="U33" s="83"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="95"/>
+      <c r="H33" s="95"/>
+      <c r="I33" s="95"/>
+      <c r="J33" s="95"/>
+      <c r="K33" s="95"/>
+      <c r="L33" s="95"/>
+      <c r="M33" s="95"/>
+      <c r="N33" s="95"/>
+      <c r="O33" s="95"/>
+      <c r="P33" s="95"/>
+      <c r="Q33" s="95"/>
+      <c r="R33" s="95"/>
+      <c r="S33" s="95"/>
+      <c r="T33" s="95"/>
+      <c r="U33" s="96"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="69"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="70"/>
-      <c r="T34" s="70"/>
-      <c r="U34" s="71"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="85"/>
+      <c r="L34" s="85"/>
+      <c r="M34" s="85"/>
+      <c r="N34" s="85"/>
+      <c r="O34" s="85"/>
+      <c r="P34" s="85"/>
+      <c r="Q34" s="85"/>
+      <c r="R34" s="85"/>
+      <c r="S34" s="85"/>
+      <c r="T34" s="85"/>
+      <c r="U34" s="86"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="69"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="70"/>
-      <c r="N35" s="70"/>
-      <c r="O35" s="70"/>
-      <c r="P35" s="70"/>
-      <c r="Q35" s="70"/>
-      <c r="R35" s="70"/>
-      <c r="S35" s="70"/>
-      <c r="T35" s="70"/>
-      <c r="U35" s="71"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="85"/>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="85"/>
+      <c r="L35" s="85"/>
+      <c r="M35" s="85"/>
+      <c r="N35" s="85"/>
+      <c r="O35" s="85"/>
+      <c r="P35" s="85"/>
+      <c r="Q35" s="85"/>
+      <c r="R35" s="85"/>
+      <c r="S35" s="85"/>
+      <c r="T35" s="85"/>
+      <c r="U35" s="86"/>
     </row>
     <row r="36" spans="1:25" s="18" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="72"/>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="73"/>
-      <c r="G36" s="73"/>
-      <c r="H36" s="73"/>
-      <c r="I36" s="73"/>
-      <c r="J36" s="73"/>
-      <c r="K36" s="73"/>
-      <c r="L36" s="73"/>
-      <c r="M36" s="73"/>
-      <c r="N36" s="73"/>
-      <c r="O36" s="73"/>
-      <c r="P36" s="73"/>
-      <c r="Q36" s="73"/>
-      <c r="R36" s="73"/>
-      <c r="S36" s="73"/>
-      <c r="T36" s="73"/>
-      <c r="U36" s="74"/>
+      <c r="A36" s="87"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="88"/>
+      <c r="G36" s="88"/>
+      <c r="H36" s="88"/>
+      <c r="I36" s="88"/>
+      <c r="J36" s="88"/>
+      <c r="K36" s="88"/>
+      <c r="L36" s="88"/>
+      <c r="M36" s="88"/>
+      <c r="N36" s="88"/>
+      <c r="O36" s="88"/>
+      <c r="P36" s="88"/>
+      <c r="Q36" s="88"/>
+      <c r="R36" s="88"/>
+      <c r="S36" s="88"/>
+      <c r="T36" s="88"/>
+      <c r="U36" s="89"/>
       <c r="W36" s="21"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="22"/>
@@ -2866,59 +3049,59 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G38" s="62">
+        <v>2</v>
+      </c>
+      <c r="G38" s="61">
         <v>152</v>
       </c>
-      <c r="H38" s="66">
+      <c r="H38" s="65">
         <v>153</v>
       </c>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="63"/>
-      <c r="L38" s="63"/>
-      <c r="M38" s="63"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="63"/>
-      <c r="R38" s="63"/>
-      <c r="S38" s="63"/>
-      <c r="T38" s="63"/>
-      <c r="U38" s="63"/>
-      <c r="V38" s="63"/>
-      <c r="W38" s="63"/>
-      <c r="X38" s="63"/>
-      <c r="Y38" s="63"/>
+      <c r="I38" s="67"/>
+      <c r="J38" s="67"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="62"/>
+      <c r="N38" s="62"/>
+      <c r="O38" s="62"/>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="62"/>
+      <c r="R38" s="62"/>
+      <c r="S38" s="62"/>
+      <c r="T38" s="62"/>
+      <c r="U38" s="62"/>
+      <c r="V38" s="62"/>
+      <c r="W38" s="62"/>
+      <c r="X38" s="62"/>
+      <c r="Y38" s="62"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="F39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G39" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="61" t="s">
+      <c r="H39" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="I39" s="64"/>
-      <c r="J39" s="64"/>
-      <c r="K39" s="64"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="64"/>
-      <c r="N39" s="64"/>
-      <c r="O39" s="64"/>
-      <c r="P39" s="64"/>
-      <c r="Q39" s="64"/>
-      <c r="R39" s="64"/>
-      <c r="S39" s="64"/>
-      <c r="T39" s="64"/>
-      <c r="U39" s="64"/>
-      <c r="V39" s="64"/>
-      <c r="W39" s="64"/>
-      <c r="X39" s="64"/>
-      <c r="Y39" s="64"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="63"/>
+      <c r="K39" s="63"/>
+      <c r="L39" s="63"/>
+      <c r="M39" s="63"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="63"/>
+      <c r="P39" s="63"/>
+      <c r="Q39" s="63"/>
+      <c r="R39" s="63"/>
+      <c r="S39" s="63"/>
+      <c r="T39" s="63"/>
+      <c r="U39" s="63"/>
+      <c r="V39" s="63"/>
+      <c r="W39" s="63"/>
+      <c r="X39" s="63"/>
+      <c r="Y39" s="63"/>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="W40" s="1"/>
@@ -2931,19 +3114,7 @@
       <c r="Y41" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="A3:U4"/>
-    <mergeCell ref="U27:U32"/>
-    <mergeCell ref="Q27:Q32"/>
-    <mergeCell ref="K27:K32"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="N27:N32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="J27:J32"/>
+  <mergeCells count="25">
     <mergeCell ref="A35:U35"/>
     <mergeCell ref="A36:U36"/>
     <mergeCell ref="T27:T32"/>
@@ -2956,6 +3127,19 @@
     <mergeCell ref="L27:L32"/>
     <mergeCell ref="A33:U33"/>
     <mergeCell ref="A34:U34"/>
+    <mergeCell ref="U27:U32"/>
+    <mergeCell ref="Q27:Q32"/>
+    <mergeCell ref="K27:K32"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="N27:N32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="J27:J32"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D39:E39 I39:Y39">
@@ -2969,7 +3153,7 @@
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6:P26">
+  <conditionalFormatting sqref="E11:G11 F6:P6 E9:E10 G7:P9 E16:P16 E12:F12 H12:P12 I10:P11 E13:H14 J14:P14 L13:P13 E15:I15 N15:P15 E18:P26 E17:N17 P17">
     <cfRule type="cellIs" dxfId="2" priority="11" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>

</xml_diff>

<commit_message>
linked .js in body, changed .js file name to index.js, updated project manager template
</commit_message>
<xml_diff>
--- a/docs/Project Manager Template.xlsx
+++ b/docs/Project Manager Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psnpo\Documents\GitHub\video-player\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D09912-BC1E-4A67-992B-E5A66D7BB33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2DAD8B-1746-4148-9617-9EA42D3BF5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Major Tasks</t>
   </si>
@@ -1193,154 +1193,154 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="37" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="50" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1967,7 +1967,7 @@
   <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="73" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2020,57 +2020,57 @@
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="101"/>
-      <c r="E3" s="102" t="s">
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="98"/>
+      <c r="F3" s="108"/>
+      <c r="G3" s="108"/>
+      <c r="H3" s="108"/>
+      <c r="I3" s="108"/>
+      <c r="J3" s="108"/>
+      <c r="K3" s="108"/>
+      <c r="L3" s="108"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="70"/>
       <c r="W3" s="13"/>
       <c r="X3" s="14"/>
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="103"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="103"/>
-      <c r="M4" s="103"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="103"/>
-      <c r="P4" s="103"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="100"/>
+      <c r="A4" s="106"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
+      <c r="N4" s="109"/>
+      <c r="O4" s="109"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="71"/>
+      <c r="R4" s="71"/>
+      <c r="S4" s="71"/>
+      <c r="T4" s="71"/>
+      <c r="U4" s="72"/>
       <c r="W4" s="16"/>
       <c r="X4" s="17"/>
       <c r="Y4" s="17"/>
@@ -2082,27 +2082,27 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="105" t="s">
+      <c r="E5" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="83" t="s">
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
+      <c r="L5" s="100"/>
+      <c r="M5" s="100"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="102"/>
+      <c r="Q5" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="80"/>
-      <c r="S5" s="80"/>
-      <c r="T5" s="80"/>
-      <c r="U5" s="82"/>
+      <c r="R5" s="100"/>
+      <c r="S5" s="100"/>
+      <c r="T5" s="100"/>
+      <c r="U5" s="102"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -2116,10 +2116,10 @@
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="107" t="s">
+      <c r="E6" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="104"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
@@ -2148,10 +2148,10 @@
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
-      <c r="E7" s="108" t="s">
+      <c r="E7" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="109" t="s">
+      <c r="F7" s="77" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="38"/>
@@ -2166,7 +2166,9 @@
       <c r="P7" s="39"/>
       <c r="Q7" s="40"/>
       <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
+      <c r="S7" s="77" t="s">
+        <v>5</v>
+      </c>
       <c r="T7" s="41"/>
       <c r="U7" s="42"/>
       <c r="W7" s="32"/>
@@ -2182,10 +2184,10 @@
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
-      <c r="E8" s="108" t="s">
+      <c r="E8" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="109" t="s">
+      <c r="F8" s="77" t="s">
         <v>5</v>
       </c>
       <c r="G8" s="38"/>
@@ -2200,7 +2202,9 @@
       <c r="P8" s="39"/>
       <c r="Q8" s="40"/>
       <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
+      <c r="S8" s="77" t="s">
+        <v>5</v>
+      </c>
       <c r="T8" s="41"/>
       <c r="U8" s="42"/>
       <c r="W8" s="32"/>
@@ -2216,8 +2220,8 @@
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="109" t="s">
+      <c r="E9" s="74"/>
+      <c r="F9" s="77" t="s">
         <v>5</v>
       </c>
       <c r="G9" s="38"/>
@@ -2249,13 +2253,13 @@
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
       <c r="E10" s="37"/>
-      <c r="F10" s="109" t="s">
+      <c r="F10" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="109" t="s">
+      <c r="G10" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="109" t="s">
+      <c r="H10" s="77" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="38"/>
@@ -2287,7 +2291,7 @@
       <c r="E11" s="37"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
-      <c r="H11" s="109" t="s">
+      <c r="H11" s="77" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="38"/>
@@ -2318,7 +2322,7 @@
       <c r="D12" s="36"/>
       <c r="E12" s="37"/>
       <c r="F12" s="38"/>
-      <c r="G12" s="109" t="s">
+      <c r="G12" s="77" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="38"/>
@@ -2352,13 +2356,13 @@
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="109" t="s">
+      <c r="I13" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="109" t="s">
+      <c r="J13" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="K13" s="109" t="s">
+      <c r="K13" s="77" t="s">
         <v>5</v>
       </c>
       <c r="L13" s="38"/>
@@ -2388,7 +2392,7 @@
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
-      <c r="I14" s="109" t="s">
+      <c r="I14" s="77" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="38"/>
@@ -2421,16 +2425,16 @@
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
       <c r="I15" s="38"/>
-      <c r="J15" s="109" t="s">
+      <c r="J15" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="109" t="s">
+      <c r="K15" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="109" t="s">
+      <c r="L15" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="M15" s="109" t="s">
+      <c r="M15" s="77" t="s">
         <v>5</v>
       </c>
       <c r="N15" s="38"/>
@@ -2492,7 +2496,7 @@
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
       <c r="N17" s="38"/>
-      <c r="O17" s="109" t="s">
+      <c r="O17" s="77" t="s">
         <v>5</v>
       </c>
       <c r="P17" s="39"/>
@@ -2760,55 +2764,55 @@
       <c r="B27" s="55"/>
       <c r="C27" s="56"/>
       <c r="D27" s="56"/>
-      <c r="E27" s="78" t="s">
+      <c r="E27" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="76" t="s">
+      <c r="F27" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="76" t="s">
+      <c r="G27" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="76" t="s">
+      <c r="H27" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="76" t="s">
+      <c r="I27" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="J27" s="76" t="s">
+      <c r="J27" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="K27" s="76" t="s">
+      <c r="K27" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="L27" s="76" t="s">
+      <c r="L27" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="M27" s="76" t="s">
+      <c r="M27" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="N27" s="76" t="s">
+      <c r="N27" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="O27" s="76" t="s">
+      <c r="O27" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="P27" s="92" t="s">
+      <c r="P27" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="Q27" s="74" t="s">
+      <c r="Q27" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="R27" s="90" t="s">
+      <c r="R27" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="S27" s="90" t="s">
+      <c r="S27" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="T27" s="90" t="s">
+      <c r="T27" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="U27" s="72" t="s">
+      <c r="U27" s="93" t="s">
         <v>37</v>
       </c>
       <c r="W27" s="32"/>
@@ -2820,23 +2824,23 @@
       <c r="B28" s="57"/>
       <c r="C28" s="56"/>
       <c r="D28" s="56"/>
-      <c r="E28" s="78"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="76"/>
-      <c r="H28" s="76"/>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="92"/>
-      <c r="Q28" s="74"/>
-      <c r="R28" s="90"/>
-      <c r="S28" s="90"/>
-      <c r="T28" s="90"/>
-      <c r="U28" s="72"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
+      <c r="K28" s="86"/>
+      <c r="L28" s="86"/>
+      <c r="M28" s="86"/>
+      <c r="N28" s="86"/>
+      <c r="O28" s="86"/>
+      <c r="P28" s="88"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="84"/>
+      <c r="S28" s="84"/>
+      <c r="T28" s="84"/>
+      <c r="U28" s="93"/>
       <c r="W28" s="32"/>
       <c r="X28" s="33"/>
       <c r="Y28" s="33"/>
@@ -2846,23 +2850,23 @@
       <c r="B29" s="57"/>
       <c r="C29" s="56"/>
       <c r="D29" s="56"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="76"/>
-      <c r="O29" s="76"/>
-      <c r="P29" s="92"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="90"/>
-      <c r="S29" s="90"/>
-      <c r="T29" s="90"/>
-      <c r="U29" s="72"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
+      <c r="I29" s="86"/>
+      <c r="J29" s="86"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
+      <c r="P29" s="88"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="84"/>
+      <c r="S29" s="84"/>
+      <c r="T29" s="84"/>
+      <c r="U29" s="93"/>
       <c r="W29" s="32"/>
       <c r="X29" s="33"/>
       <c r="Y29" s="33"/>
@@ -2872,23 +2876,23 @@
       <c r="B30" s="58"/>
       <c r="C30" s="56"/>
       <c r="D30" s="56"/>
-      <c r="E30" s="78"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76"/>
-      <c r="P30" s="92"/>
-      <c r="Q30" s="74"/>
-      <c r="R30" s="90"/>
-      <c r="S30" s="90"/>
-      <c r="T30" s="90"/>
-      <c r="U30" s="72"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="86"/>
+      <c r="G30" s="86"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="86"/>
+      <c r="J30" s="86"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="86"/>
+      <c r="M30" s="86"/>
+      <c r="N30" s="86"/>
+      <c r="O30" s="86"/>
+      <c r="P30" s="88"/>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="84"/>
+      <c r="S30" s="84"/>
+      <c r="T30" s="84"/>
+      <c r="U30" s="93"/>
       <c r="X30" s="33"/>
       <c r="Y30" s="33"/>
     </row>
@@ -2897,23 +2901,23 @@
       <c r="B31" s="55"/>
       <c r="C31" s="56"/>
       <c r="D31" s="56"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="76"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="76"/>
-      <c r="P31" s="92"/>
-      <c r="Q31" s="74"/>
-      <c r="R31" s="90"/>
-      <c r="S31" s="90"/>
-      <c r="T31" s="90"/>
-      <c r="U31" s="72"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="86"/>
+      <c r="G31" s="86"/>
+      <c r="H31" s="86"/>
+      <c r="I31" s="86"/>
+      <c r="J31" s="86"/>
+      <c r="K31" s="86"/>
+      <c r="L31" s="86"/>
+      <c r="M31" s="86"/>
+      <c r="N31" s="86"/>
+      <c r="O31" s="86"/>
+      <c r="P31" s="88"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="84"/>
+      <c r="S31" s="84"/>
+      <c r="T31" s="84"/>
+      <c r="U31" s="93"/>
       <c r="X31" s="33"/>
       <c r="Y31" s="33"/>
     </row>
@@ -2922,118 +2926,118 @@
       <c r="B32" s="59"/>
       <c r="C32" s="56"/>
       <c r="D32" s="56"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="77"/>
-      <c r="J32" s="77"/>
-      <c r="K32" s="77"/>
-      <c r="L32" s="77"/>
-      <c r="M32" s="77"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="77"/>
-      <c r="P32" s="93"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="91"/>
-      <c r="S32" s="91"/>
-      <c r="T32" s="91"/>
-      <c r="U32" s="73"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="87"/>
+      <c r="K32" s="87"/>
+      <c r="L32" s="87"/>
+      <c r="M32" s="87"/>
+      <c r="N32" s="87"/>
+      <c r="O32" s="87"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="85"/>
+      <c r="S32" s="85"/>
+      <c r="T32" s="85"/>
+      <c r="U32" s="94"/>
       <c r="W32" s="21"/>
       <c r="X32" s="21"/>
       <c r="Y32" s="21"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33" s="94"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
-      <c r="K33" s="95"/>
-      <c r="L33" s="95"/>
-      <c r="M33" s="95"/>
-      <c r="N33" s="95"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="95"/>
-      <c r="S33" s="95"/>
-      <c r="T33" s="95"/>
-      <c r="U33" s="96"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="91"/>
+      <c r="P33" s="91"/>
+      <c r="Q33" s="91"/>
+      <c r="R33" s="91"/>
+      <c r="S33" s="91"/>
+      <c r="T33" s="91"/>
+      <c r="U33" s="92"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34" s="84"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="85"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
-      <c r="I34" s="85"/>
-      <c r="J34" s="85"/>
-      <c r="K34" s="85"/>
-      <c r="L34" s="85"/>
-      <c r="M34" s="85"/>
-      <c r="N34" s="85"/>
-      <c r="O34" s="85"/>
-      <c r="P34" s="85"/>
-      <c r="Q34" s="85"/>
-      <c r="R34" s="85"/>
-      <c r="S34" s="85"/>
-      <c r="T34" s="85"/>
-      <c r="U34" s="86"/>
+      <c r="A34" s="78"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="79"/>
+      <c r="P34" s="79"/>
+      <c r="Q34" s="79"/>
+      <c r="R34" s="79"/>
+      <c r="S34" s="79"/>
+      <c r="T34" s="79"/>
+      <c r="U34" s="80"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35" s="84"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="85"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="85"/>
-      <c r="J35" s="85"/>
-      <c r="K35" s="85"/>
-      <c r="L35" s="85"/>
-      <c r="M35" s="85"/>
-      <c r="N35" s="85"/>
-      <c r="O35" s="85"/>
-      <c r="P35" s="85"/>
-      <c r="Q35" s="85"/>
-      <c r="R35" s="85"/>
-      <c r="S35" s="85"/>
-      <c r="T35" s="85"/>
-      <c r="U35" s="86"/>
+      <c r="A35" s="78"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="79"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="79"/>
+      <c r="T35" s="79"/>
+      <c r="U35" s="80"/>
     </row>
     <row r="36" spans="1:25" s="18" customFormat="1" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="87"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="88"/>
-      <c r="D36" s="88"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="88"/>
-      <c r="I36" s="88"/>
-      <c r="J36" s="88"/>
-      <c r="K36" s="88"/>
-      <c r="L36" s="88"/>
-      <c r="M36" s="88"/>
-      <c r="N36" s="88"/>
-      <c r="O36" s="88"/>
-      <c r="P36" s="88"/>
-      <c r="Q36" s="88"/>
-      <c r="R36" s="88"/>
-      <c r="S36" s="88"/>
-      <c r="T36" s="88"/>
-      <c r="U36" s="89"/>
+      <c r="A36" s="81"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="82"/>
+      <c r="O36" s="82"/>
+      <c r="P36" s="82"/>
+      <c r="Q36" s="82"/>
+      <c r="R36" s="82"/>
+      <c r="S36" s="82"/>
+      <c r="T36" s="82"/>
+      <c r="U36" s="83"/>
       <c r="W36" s="21"/>
       <c r="X36" s="22"/>
       <c r="Y36" s="22"/>
@@ -3115,6 +3119,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="N27:N32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="J27:J32"/>
     <mergeCell ref="A35:U35"/>
     <mergeCell ref="A36:U36"/>
     <mergeCell ref="T27:T32"/>
@@ -3131,15 +3144,6 @@
     <mergeCell ref="Q27:Q32"/>
     <mergeCell ref="K27:K32"/>
     <mergeCell ref="E27:E32"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="N27:N32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="J27:J32"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:P4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D39:E39 I39:Y39">
@@ -3153,7 +3157,7 @@
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:G11 F6:P6 E9:E10 G7:P9 E16:P16 E12:F12 H12:P12 I10:P11 E13:H14 J14:P14 L13:P13 E15:I15 N15:P15 E18:P26 E17:N17 P17">
+  <conditionalFormatting sqref="F6:P6 G7:P9 E9:E10 I10:P11 E11:G11 E12:F12 H12:P12 L13:P13 E13:H14 J14:P14 E15:I15 N15:P15 E16:P16 E17:N17 P17 E18:P26">
     <cfRule type="cellIs" dxfId="2" priority="11" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>

</xml_diff>